<commit_message>
Controller improved for Iphone (still not perfect)
</commit_message>
<xml_diff>
--- a/GlyphPosition.xlsx
+++ b/GlyphPosition.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -755,7 +754,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G11"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,19 +767,19 @@
         <v>104</v>
       </c>
       <c r="C1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D1">
         <f>ROUND(A1*$C$1,0)</f>
-        <v>216</v>
+        <v>144</v>
       </c>
       <c r="E1">
         <f>ROUND(B1*$C$1,0)</f>
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G1" t="str">
         <f>"{x: "&amp;D1&amp;", y: "&amp;E1&amp;"},"</f>
-        <v>{x: 216, y: 31},</v>
+        <v>{x: 144, y: 21},</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -792,15 +791,15 @@
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D11" si="0">ROUND(A2*$C$1,0)</f>
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E11" si="1">ROUND(B2*$C$1,0)</f>
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G11" si="2">"{x: "&amp;D2&amp;", y: "&amp;E2&amp;"},"</f>
-        <v>{x: 47, y: 129},</v>
+        <f t="shared" ref="G2:G10" si="2">"{x: "&amp;D2&amp;", y: "&amp;E2&amp;"},"</f>
+        <v>{x: 31, y: 86},</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,15 +811,15 @@
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
-        <v>324</v>
+        <v>216</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 47, y: 324},</v>
+        <v>{x: 31, y: 216},</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,15 +831,15 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>216</v>
+        <v>144</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>422</v>
+        <v>281</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 216, y: 422},</v>
+        <v>{x: 144, y: 281},</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -852,15 +851,15 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>384</v>
+        <v>256</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>324</v>
+        <v>216</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 384, y: 324},</v>
+        <v>{x: 256, y: 216},</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -872,15 +871,15 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>385</v>
+        <v>257</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 385, y: 129},</v>
+        <v>{x: 257, y: 86},</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -892,15 +891,15 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>177</v>
+        <v>118</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 131, y: 177},</v>
+        <v>{x: 87, y: 118},</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -912,15 +911,15 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>275</v>
+        <v>183</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 132, y: 275},</v>
+        <v>{x: 88, y: 183},</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -932,15 +931,15 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>275</v>
+        <v>184</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 300, y: 275},</v>
+        <v>{x: 200, y: 184},</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -952,15 +951,15 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="2"/>
-        <v>{x: 300, y: 178},</v>
+        <v>{x: 200, y: 119},</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,15 +971,15 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>216</v>
+        <v>144</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>226</v>
+        <v>151</v>
       </c>
       <c r="G11" t="str">
         <f>"{x: "&amp;D11&amp;", y: "&amp;E11&amp;"}"</f>
-        <v>{x: 216, y: 226}</v>
+        <v>{x: 144, y: 151}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>